<commit_message>
User Mobility: - code refactoring - added new user class - fixed excel group reading issue
</commit_message>
<xml_diff>
--- a/Checkpoint_User_Mobility/User-Mobility-Test.xlsx
+++ b/Checkpoint_User_Mobility/User-Mobility-Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_User_Mobility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBD7B03-EF21-4CCE-8E48-565C4E811A29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CA7B27-C842-4E41-AF0E-B8D605E5AADF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>User Email</t>
   </si>
@@ -39,7 +39,10 @@
     <t>Action</t>
   </si>
   <si>
-    <t>delete</t>
+    <t>add</t>
+  </si>
+  <si>
+    <t>mhemaraju@auchan.com</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,8 +459,12 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
@@ -466,6 +473,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7C204F65-3DA0-4A96-B650-E75F8C5E34EE}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{CC3477BC-D85C-48D0-9C39-A00340EA6BCE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>